<commit_message>
Schema Changes for eCitation - Removed Signature, changed "City Relief" to "Civil Relief", removed MTOM attachment.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/service-specifications/Court_Case_Filing_Service/artifacts/service_model/information_model/Court_Case_Filing-IEPD/documentation/impl-artifacts/vermont/Citation_Case_Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/service-specifications/Court_Case_Filing_Service/artifacts/service_model/information_model/Court_Case_Filing-IEPD/documentation/impl-artifacts/vermont/Citation_Case_Mapping.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6000" yWindow="880" windowWidth="20880" windowHeight="15880"/>
+    <workbookView xWindow="6000" yWindow="880" windowWidth="30440" windowHeight="15880"/>
   </bookViews>
   <sheets>
     <sheet name="eCitation" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="284">
   <si>
     <t>Description</t>
   </si>
@@ -180,9 +180,6 @@
     <t>Officer Name</t>
   </si>
   <si>
-    <t>Officer Signature</t>
-  </si>
-  <si>
     <t>Dept No.</t>
   </si>
   <si>
@@ -372,15 +369,6 @@
     <t>Officer Badge Number</t>
   </si>
   <si>
-    <t>City Relief Act Indicator</t>
-  </si>
-  <si>
-    <t>City Relief Act Juvenile Indicator</t>
-  </si>
-  <si>
-    <t>City Relief Act Other Indicator</t>
-  </si>
-  <si>
     <t>Weight Unit</t>
   </si>
   <si>
@@ -490,9 +478,6 @@
   </si>
   <si>
     <t>05401-2277</t>
-  </si>
-  <si>
-    <t>City Relief Act Other Text</t>
   </si>
   <si>
     <t>Commerical Vehicle Indicator</t>
@@ -649,9 +634,6 @@
 (Elements in RED are OJB extensions to ECF)</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>ECF Mapping</t>
   </si>
   <si>
@@ -812,18 +794,6 @@
     <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/ojb-cit-ext:DrivingIncidentAugmentation/ojb-cit-ext:SeatBeltViolationIndicator</t>
   </si>
   <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/ojb-cit-ext:DrivingIncidentAugmentation/ojb-cit-ext:CityReliefActIndicator</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/ojb-cit-ext:DrivingIncidentAugmentation/ojb-cit-ext:CityReliefActJuvenileIndicator</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/ojb-cit-ext:DrivingIncidentAugmentation/ojb-cit-ext:CityReliefActOtherIndicator</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/ojb-cit-ext:DrivingIncidentAugmentation/ojb-cit-ext:CityReliefActOtherText</t>
-  </si>
-  <si>
     <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Offense/j:Statute/j:StatuteCodeIdentification/nc:IdentificationID</t>
   </si>
   <si>
@@ -879,6 +849,30 @@
   </si>
   <si>
     <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/ojb-cit-ext:PersonDriverLicense/ojb-cit-ext:DriverLicenseCDLIndicator</t>
+  </si>
+  <si>
+    <t>Civil Relief Act Indicator</t>
+  </si>
+  <si>
+    <t>Civil Relief Act Juvenile Indicator</t>
+  </si>
+  <si>
+    <t>Civil Relief Act Other Indicator</t>
+  </si>
+  <si>
+    <t>Civil Relief Act Other Text</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/ojb-cit-ext:DrivingIncidentAugmentation/ojb-cit-ext:CivilReliefActIndicator</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/ojb-cit-ext:DrivingIncidentAugmentation/ojb-cit-ext:CivilReliefActJuvenileIndicator</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/ojb-cit-ext:DrivingIncidentAugmentation/ojb-cit-ext:CivilReliefActOtherIndicator</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/ojb-cit-ext:DrivingIncidentAugmentation/ojb-cit-ext:CivilReliefActOtherText</t>
   </si>
 </sst>
 </file>
@@ -2902,11 +2896,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E87"/>
+  <dimension ref="A1:E86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomLeft" activeCell="A75" sqref="A75:XFD75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2922,53 +2916,53 @@
   <sheetData>
     <row r="1" spans="1:5" s="9" customFormat="1" ht="28">
       <c r="A1" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="19" customHeight="1">
       <c r="A2" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" ht="28">
       <c r="A3" s="14" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="D3" s="2">
         <v>82734800</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="3" customFormat="1">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A4" s="3" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>48</v>
@@ -2977,7 +2971,7 @@
         <v>42304</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="3" customFormat="1" ht="28">
@@ -2985,7 +2979,7 @@
         <v>47</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>47</v>
@@ -2994,15 +2988,15 @@
         <v>105</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A6" s="6" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>49</v>
@@ -3011,15 +3005,15 @@
         <v>1</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A7" s="6" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>50</v>
@@ -3028,58 +3022,58 @@
         <v>0</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" ht="28">
       <c r="A9" s="15" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="10" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" ht="28">
+    <row r="11" spans="1:5" ht="42">
       <c r="A11" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -3088,19 +3082,19 @@
     </row>
     <row r="13" spans="1:5" ht="42">
       <c r="A13" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="42">
@@ -3114,47 +3108,47 @@
         <v>12</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="42">
       <c r="A15" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="56">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="70">
       <c r="A16" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="42">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="56">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
@@ -3165,13 +3159,13 @@
         <v>4</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="56">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="70">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
@@ -3182,13 +3176,13 @@
         <v>5</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" s="3" customFormat="1" ht="42">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="3" customFormat="1" ht="56">
       <c r="A19" s="3" t="s">
         <v>6</v>
       </c>
@@ -3199,13 +3193,13 @@
         <v>6</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="42">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="56">
       <c r="A20" s="14" t="s">
         <v>1</v>
       </c>
@@ -3219,32 +3213,32 @@
         <v>41444812</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="42">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="56">
       <c r="A21" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="42">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="56">
       <c r="A22" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>10</v>
@@ -3253,15 +3247,15 @@
         <v>12345678</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" s="3" customFormat="1" ht="84">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="3" customFormat="1" ht="98">
       <c r="A23" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>15</v>
@@ -3270,15 +3264,15 @@
         <v>8023631111</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" s="3" customFormat="1" ht="84">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" s="3" customFormat="1" ht="98">
       <c r="A24" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>16</v>
@@ -3287,7 +3281,7 @@
         <v>8023631112</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="3" customFormat="1" ht="42">
@@ -3304,41 +3298,41 @@
         <v>24014</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A26" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="3" customFormat="1" ht="56">
       <c r="A27" s="16" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="3" customFormat="1" ht="42">
@@ -3352,21 +3346,21 @@
         <v>19</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A29" s="3" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="3" customFormat="1" ht="42">
@@ -3383,57 +3377,57 @@
         <v>135</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A31" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A32" s="3" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A33" s="3" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -3442,58 +3436,58 @@
     </row>
     <row r="35" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A35" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="3" customFormat="1" ht="56">
       <c r="A36" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="3" customFormat="1" ht="56">
       <c r="A37" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A38" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>23</v>
@@ -3502,66 +3496,66 @@
         <v>2015</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A39" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A40" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A41" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A42" s="16" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>38</v>
@@ -3570,15 +3564,15 @@
         <v>0</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" s="3" customFormat="1" ht="42">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" s="3" customFormat="1" ht="56">
       <c r="A43" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>39</v>
@@ -3587,12 +3581,12 @@
         <v>0</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
@@ -3601,109 +3595,109 @@
     </row>
     <row r="45" spans="1:5" s="3" customFormat="1" ht="68" customHeight="1">
       <c r="A45" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="46" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A46" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E46" s="15" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
     </row>
     <row r="47" spans="1:5" s="3" customFormat="1" ht="56">
       <c r="A47" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E47" s="15" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="48" spans="1:5" s="3" customFormat="1" ht="56">
       <c r="A48" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E48" s="15" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
     </row>
     <row r="49" spans="1:5" s="3" customFormat="1" ht="56">
       <c r="A49" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E49" s="15" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
     </row>
     <row r="50" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A50" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E50" s="15" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" s="3" customFormat="1">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A51" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>32</v>
@@ -3712,7 +3706,7 @@
         <v>0.2</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
     </row>
     <row r="52" spans="1:5" s="3" customFormat="1" ht="56">
@@ -3720,7 +3714,7 @@
         <v>33</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>33</v>
@@ -3729,21 +3723,21 @@
         <v>30</v>
       </c>
       <c r="E52" s="15" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="53" spans="1:5" s="3" customFormat="1" ht="56">
       <c r="A53" s="3" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="E53" s="15" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
     </row>
     <row r="54" spans="1:5" s="3" customFormat="1" ht="42">
@@ -3751,7 +3745,7 @@
         <v>34</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>34</v>
@@ -3760,29 +3754,29 @@
         <v>40</v>
       </c>
       <c r="E54" s="15" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="55" spans="1:5" s="3" customFormat="1" ht="56">
       <c r="A55" s="3" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="E55" s="15" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
     <row r="56" spans="1:5" s="3" customFormat="1" ht="56">
       <c r="A56" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>35</v>
@@ -3791,15 +3785,15 @@
         <v>0</v>
       </c>
       <c r="E56" s="15" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" s="3" customFormat="1" ht="42">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" s="3" customFormat="1" ht="56">
       <c r="A57" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>36</v>
@@ -3808,15 +3802,15 @@
         <v>0</v>
       </c>
       <c r="E57" s="15" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" s="3" customFormat="1" ht="42">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" s="3" customFormat="1" ht="56">
       <c r="A58" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>37</v>
@@ -3825,77 +3819,77 @@
         <v>0</v>
       </c>
       <c r="E58" s="15" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="42">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="56">
       <c r="A59" s="12" t="s">
-        <v>117</v>
+        <v>276</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D59" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E59" s="15" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="42">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="56">
       <c r="A60" s="12" t="s">
-        <v>118</v>
+        <v>277</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D60" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E60" s="15" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="42">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="56">
       <c r="A61" s="12" t="s">
-        <v>119</v>
+        <v>278</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D61" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E61" s="15" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="42">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="56">
       <c r="A62" s="12" t="s">
-        <v>157</v>
+        <v>279</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E62" s="15" t="s">
-        <v>266</v>
+        <v>283</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
@@ -3904,95 +3898,95 @@
     </row>
     <row r="64" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A64" s="6" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
     </row>
     <row r="65" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A65" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
     </row>
     <row r="66" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A66" s="6" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
     </row>
     <row r="67" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A67" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>43</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" s="3" customFormat="1">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A68" s="6" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D68" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" s="3" customFormat="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A69" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>44</v>
@@ -4001,15 +3995,15 @@
         <v>2</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" s="3" customFormat="1">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A70" s="6" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>45</v>
@@ -4018,15 +4012,15 @@
         <v>47</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" s="3" customFormat="1">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A71" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>46</v>
@@ -4035,19 +4029,19 @@
         <v>1197</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
       <c r="E72" s="5"/>
     </row>
-    <row r="73" spans="1:5" s="3" customFormat="1" ht="42">
+    <row r="73" spans="1:5" s="3" customFormat="1" ht="56">
       <c r="A73" s="3" t="s">
         <v>52</v>
       </c>
@@ -4058,18 +4052,18 @@
         <v>52</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
     </row>
     <row r="74" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A74" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>51</v>
@@ -4078,205 +4072,191 @@
         <v>12345</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" s="3" customFormat="1">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A75" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B75" s="6" t="s">
-        <v>53</v>
+        <v>138</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>138</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E75" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" s="3" customFormat="1" ht="42">
+      <c r="D75" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A76" s="3" t="s">
-        <v>142</v>
+        <v>54</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>142</v>
+        <v>54</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>54</v>
       </c>
       <c r="D76" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B77" s="5"/>
+      <c r="C77" s="5"/>
+      <c r="D77" s="5"/>
+      <c r="E77" s="5"/>
+    </row>
+    <row r="78" spans="1:5" ht="42">
+      <c r="A78" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="42">
+      <c r="A79" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="56">
+      <c r="A80" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="56">
+      <c r="A81" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D81" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="E76" s="3" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" s="3" customFormat="1">
-      <c r="A77" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D77" s="3" t="s">
+      <c r="E81" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="56">
+      <c r="A82" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="56">
+      <c r="A83" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D83" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E77" s="3" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5">
-      <c r="A78" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="B78" s="5"/>
-      <c r="C78" s="5"/>
-      <c r="D78" s="5"/>
-      <c r="E78" s="5"/>
-    </row>
-    <row r="79" spans="1:5" ht="28">
-      <c r="A79" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="E79" s="3" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="28">
-      <c r="A80" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E80" s="3" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" ht="42">
-      <c r="A81" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="E81" s="3" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" ht="42">
-      <c r="A82" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="E82" s="3" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" ht="42">
-      <c r="A83" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>124</v>
-      </c>
       <c r="E83" s="3" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="42">
-      <c r="A84" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="E84" s="3" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5">
-      <c r="A85" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="B85" s="5"/>
-      <c r="C85" s="5"/>
-      <c r="D85" s="5"/>
-      <c r="E85" s="5"/>
-    </row>
-    <row r="86" spans="1:5" ht="42">
-      <c r="A86" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="C86" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="B84" s="5"/>
+      <c r="C84" s="5"/>
+      <c r="D84" s="5"/>
+      <c r="E84" s="5"/>
+    </row>
+    <row r="85" spans="1:5" ht="56">
+      <c r="A85" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C85" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D86" s="2" t="b">
+      <c r="D85" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="E86" s="15" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" ht="119" customHeight="1">
-      <c r="A87" s="17" t="s">
-        <v>211</v>
-      </c>
-      <c r="B87" s="18"/>
-      <c r="C87" s="18"/>
-      <c r="D87" s="18"/>
+      <c r="E85" s="15" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="119" customHeight="1">
+      <c r="A86" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="B86" s="18"/>
+      <c r="C86" s="18"/>
+      <c r="D86" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A87:D87"/>
+    <mergeCell ref="A86:D86"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Removed TrafficIncidentAccidentIndicator extension element.  Updated mapping spreadsheets.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/service-specifications/Court_Case_Filing_Service/artifacts/service_model/information_model/Court_Case_Filing-IEPD/documentation/impl-artifacts/vermont/Citation_Case_Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/service-specifications/Court_Case_Filing_Service/artifacts/service_model/information_model/Court_Case_Filing-IEPD/documentation/impl-artifacts/vermont/Citation_Case_Mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6000" yWindow="880" windowWidth="30440" windowHeight="15880"/>
+    <workbookView xWindow="-28460" yWindow="5920" windowWidth="30440" windowHeight="15880"/>
   </bookViews>
   <sheets>
     <sheet name="eCitation" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="288">
   <si>
     <t>Description</t>
   </si>
@@ -641,216 +641,6 @@
 ECF extension elements are in red.</t>
   </si>
   <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/nc:ActivityIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/nc:ActivityDate/nc:Date</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/ojb-cit-ext:CitationAugmentation/ojb-cit-ext:CitationWaiverAmount</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/ojb-cit-ext:CitationAugmentation/ojb-cit-ext:CitationServedIndicator</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/ojb-cit-ext:CitationAugmentation/ojb-cit-ext:CitationMailedIndicator</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityOrganization/nc:OrganizationName</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityOrganization[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationDeliveryRecipientAssociation/nc:EntityOrganizationReference/@s:ref]/nc:OrganizationName</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonName/nc:PersonSurName</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonName/nc:PersonGivenName</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonName/nc:PersonMiddleName</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationStreet/nc:StreetFullText</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationCityName</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationCountryFIPS10-4Code</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationPostalCode</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/ojb-cit-ext:PersonDriverLicense/nc:DriverLicenseIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/ojb-cit-ext:PersonDriverLicense/nc:DriverLicenseIdentification/j:IdentificationJurisdictionNCICLISCode</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]//ojb-cit-ext:PersonAugmentation/ojb-cit-ext:PersonFishAndWildlifeLicenseIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/nc:ContactInformation/nc:ContactTelephoneNumber[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson/ojb-cit-ext:PersonAugmentation/nc:PersonContactInformationAssociation[nc:ContactInformationIsHomeIndicator="true"]/nc:ContactInformationReference/@s:ref]/nc:FullTelephoneNumber/nc:TelephoneNumberFullID</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/nc:ContactInformation/nc:ContactTelephoneNumber[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson/ojb-cit-ext:PersonAugmentation/nc:PersonContactInformationAssociation[nc:ContactInformationIsWorkIndicator="true"]/nc:ContactInformationReference/@s:ref]/nc:FullTelephoneNumber/nc:TelephoneNumberFullID</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonBirthDate/nc:Date</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonSexCode</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonBirthLocation/nc:LocationAddress/nc:StructuredAddress/nc:LocationCityName</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonHeightMeasure/nc:MeasureText</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonHeightMeasure/nc:MeasureUnitText</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonWeightMeasure/nc:MeasureText</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonWeightMeasure/nc:MeasureUnitText</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonHairColorCode</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonEyeColorCode</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/nc:VehicleIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/nc:ConveyanceRegistrationPlateIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/nc:ConveyanceRegistrationPlateIdentification/j:IdentificationJurisdictionNCICLISCode</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/nc:ItemModelYearDate</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/nc:VehicleMakeCode</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/nc:VehicleColorPrimaryCode</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/nc:VehicleStyleCode</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/nc:VehicleCMVIndicator</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/ojb-cit-ext:VehicleAugmentation/ojb-cit-ext:VehicleHazardousMaterialIndicator</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/nc:ActivityIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/nc:ActivityDate/nc:DateTime</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/nc:IncidentLocation/nc:LocationAddress/nc:StructuredAddress/nc:LocationCityName</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/nc:IncidentLocation/nc:LocationHighway/nc:HighwayID</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/nc:IncidentLocation/nc:LocationHighway/nc:HighwayPositionText</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/nc:ActivityDescriptionText</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/ecf-cit:PersonBloodAlcoholNumber</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/j:DrivingIncidentRecordedSpeedRate/nc:MeasureText</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/j:DrivingIncidentRecordedSpeedRate/nc:MeasureUnitText</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/j:DrivingIncidentLegalSpeedRate/nc:MeasureText</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/j:DrivingIncidentLegalSpeedRate/nc:MeasureUnitText</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/j:IncidentAugmentation/j:IncidentTrafficAccidentInvolvedIndicator</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/ojb-cit-ext:DrivingIncidentAugmentation/ojb-cit-ext:DrivingAccidentFatalityIndicator</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/ojb-cit-ext:DrivingIncidentAugmentation/ojb-cit-ext:SeatBeltViolationIndicator</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Offense/j:Statute/j:StatuteCodeIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Offense/ojb-cit-ext:OffenseViolatedStatute/j:StatuteCodeIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Offense/ojb-cit-ext:CFRStatute/j:StatuteCodeIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/j:CaseCharge/j:ChargeStatute/j:StatuteOffenseIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Offense/ojb-cit-ext:RelatedCriminalChargeIndicator</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Offense/ojb-cit-ext:DrivingOffensePoints</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Offense/ojb-cit-ext:OffenseFineAmountMinimum</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Offense/ojb-cit-ext:OffenseFineAmountMaximum</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/j:CitationIssuingOfficial/nc:RoleOfPersonReference/@s:ref]/nc:PersonName/nc:PersonFullName</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/j:CitationIssuingOfficial/j:EnforcementOfficialBadgeIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/j:CitationAgency/nc:OrganizationPrimaryContactInformation/nc:ContactEntity/ecf:EntityOrganization/j:OrganizationAugmentation/j:OrganizationORIIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/j:CitationAgency/nc:OrganizationName</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/nc:PersonName/nc:PersonGivenName</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/nc:PersonName/nc:PersonSurName</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/ecf:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationStreet/nc:StreetFullText</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/ecf:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationCityName</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/ecf:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationCountryFIPS10-4Code</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/ecf:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationPostalCode</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/ojb-cit-ext:PersonDriverLicense/ojb-cit-ext:DriverLicenseCDLIndicator</t>
-  </si>
-  <si>
     <t>Civil Relief Act Indicator</t>
   </si>
   <si>
@@ -863,16 +653,238 @@
     <t>Civil Relief Act Other Text</t>
   </si>
   <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/ojb-cit-ext:DrivingIncidentAugmentation/ojb-cit-ext:CivilReliefActIndicator</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/ojb-cit-ext:DrivingIncidentAugmentation/ojb-cit-ext:CivilReliefActJuvenileIndicator</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/ojb-cit-ext:DrivingIncidentAugmentation/ojb-cit-ext:CivilReliefActOtherIndicator</t>
-  </si>
-  <si>
-    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/ojb-cit-ext:DrivingIncidentAugmentation/ojb-cit-ext:CivilReliefActOtherText</t>
+    <t>Officer ID</t>
+  </si>
+  <si>
+    <t>A unique identifier assigned to an officer</t>
+  </si>
+  <si>
+    <t>ID34567</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/nc:ActivityIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/nc:ActivityDate/nc:Date</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/ojb-cit-ext:CitationAugmentation/ojb-cit-ext:CitationWaiverAmount</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/ojb-cit-ext:CitationAugmentation/ojb-cit-ext:CitationServedIndicator</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/ojb-cit-ext:CitationAugmentation/ojb-cit-ext:CitationMailedIndicator</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityOrganization/nc:OrganizationName</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityOrganization[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationDeliveryRecipientAssociation/nc:EntityOrganizationReference/@s:ref]/nc:OrganizationName</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonName/nc:PersonSurName</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonName/nc:PersonGivenName</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonName/nc:PersonMiddleName</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationStreet/nc:StreetFullText</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationCityName</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationCountryFIPS10-4Code</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationPostalCode</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/ojb-cit-ext:PersonDriverLicense/nc:DriverLicenseIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/ojb-cit-ext:PersonDriverLicense/nc:DriverLicenseIdentification/j:IdentificationJurisdictionNCICLISCode</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]//ojb-cit-ext:PersonAugmentation/ojb-cit-ext:PersonFishAndWildlifeLicenseIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/nc:ContactInformation/nc:ContactTelephoneNumber[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson/ojb-cit-ext:PersonAugmentation/nc:PersonContactInformationAssociation[nc:ContactInformationIsHomeIndicator="true"]/nc:ContactInformationReference/@s:ref]/nc:FullTelephoneNumber/nc:TelephoneNumberFullID</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/nc:ContactInformation/nc:ContactTelephoneNumber[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson/ojb-cit-ext:PersonAugmentation/nc:PersonContactInformationAssociation[nc:ContactInformationIsWorkIndicator="true"]/nc:ContactInformationReference/@s:ref]/nc:FullTelephoneNumber/nc:TelephoneNumberFullID</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonBirthDate/nc:Date</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonSexCode</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonBirthLocation/nc:LocationAddress/nc:StructuredAddress/nc:LocationCityName</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonHeightMeasure/nc:MeasureText</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonHeightMeasure/nc:MeasureUnitText</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonWeightMeasure/nc:MeasureText</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonWeightMeasure/nc:MeasureUnitText</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonHairColorCode</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonEyeColorCode</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/nc:VehicleIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/nc:ConveyanceRegistrationPlateIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/nc:ConveyanceRegistrationPlateIdentification/j:IdentificationJurisdictionNCICLISCode</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/nc:ItemModelYearDate</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/nc:VehicleMakeCode</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/nc:VehicleColorPrimaryCode</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/nc:VehicleStyleCode</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/nc:VehicleCMVIndicator</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/ojb-cit-ext:VehicleAugmentation/ojb-cit-ext:VehicleHazardousMaterialIndicator</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/nc:ActivityIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/nc:ActivityDate/nc:DateTime</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/nc:IncidentLocation/nc:LocationAddress/nc:StructuredAddress/nc:LocationCityName</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/nc:IncidentLocation/nc:LocationHighway/nc:HighwayID</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/nc:IncidentLocation/nc:LocationHighway/nc:HighwayPositionText</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/nc:ActivityDescriptionText</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/ecf-cit:PersonBloodAlcoholNumber</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/j:DrivingIncidentRecordedSpeedRate/nc:MeasureText</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/j:DrivingIncidentRecordedSpeedRate/nc:MeasureUnitText</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/j:DrivingIncidentLegalSpeedRate/nc:MeasureText</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/j:DrivingIncidentLegalSpeedRate/nc:MeasureUnitText</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/j:IncidentAugmentation/j:IncidentTrafficAccidentInvolvedIndicator</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/ojb-cit-ext:DrivingIncidentAugmentation/ojb-cit-ext:DrivingAccidentFatalityIndicator</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/ojb-cit-ext:DrivingIncidentAugmentation/ojb-cit-ext:SeatBeltViolationIndicator</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/ojb-cit-ext:DrivingIncidentAugmentation/ojb-cit-ext:CivilReliefActIndicator</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/ojb-cit-ext:DrivingIncidentAugmentation/ojb-cit-ext:CivilReliefActJuvenileIndicator</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/ojb-cit-ext:DrivingIncidentAugmentation/ojb-cit-ext:CivilReliefActOtherIndicator</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/ojb-cit-ext:DrivingIncidentAugmentation/ojb-cit-ext:CivilReliefActOtherText</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Offense/j:Statute/j:StatuteCodeIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Offense/ojb-cit-ext:OffenseViolatedStatute/j:StatuteCodeIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Offense/ojb-cit-ext:CFRStatute/j:StatuteCodeIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/j:CaseCharge/j:ChargeStatute/j:StatuteOffenseIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Offense/ojb-cit-ext:RelatedCriminalChargeIndicator</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Offense/ojb-cit-ext:DrivingOffensePoints</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Offense/ojb-cit-ext:OffenseFineAmountMinimum</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Offense/ojb-cit-ext:OffenseFineAmountMaximum</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/j:CitationAgency/nc:OrganizationPrimaryContactInformation/nc:ContactEntity/ecf:EntityOrganization/j:OrganizationAugmentation/j:OrganizationORIIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/j:CitationAgency/nc:OrganizationName</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityPerson[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/nc:PersonName/nc:PersonGivenName</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityPerson[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/nc:PersonName/nc:PersonSurName</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityPerson[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/ecf:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationStreet/nc:StreetFullText</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityPerson[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/ecf:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationCityName</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityPerson[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/ecf:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationCountryFIPS10-4Code</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityPerson[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/ecf:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationPostalCode</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/ojb-cit-ext:PersonDriverLicense/ojb-cit-ext:DriverLicenseCDLIndicator</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityPerson[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/ojb-cit-ext:CitationIssuingOfficial/nc:RoleOfPersonReference/@s:ref]/nc:PersonName/nc:PersonFullName</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/ojb-cit-ext:CitationIssuingOfficial/ojb-cit-ext:EnforcementOfficialIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/ojb-cit-ext:CitationIssuingOfficial/j:EnforcementOfficialBadgeIdentification/nc:IdentificationID</t>
   </si>
 </sst>
 </file>
@@ -1082,7 +1094,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="728">
+  <cellStyleXfs count="730">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -1109,6 +1121,8 @@
     <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1869,7 +1883,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="728">
+  <cellStyles count="730">
     <cellStyle name="Accent1 - 20%" xfId="3"/>
     <cellStyle name="Accent1 - 40%" xfId="4"/>
     <cellStyle name="Accent1 - 60%" xfId="5"/>
@@ -2242,6 +2256,7 @@
     <cellStyle name="Followed Hyperlink" xfId="723" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="725" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="727" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="729" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
@@ -2593,6 +2608,7 @@
     <cellStyle name="Hyperlink" xfId="722" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="724" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="726" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="728" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="24"/>
@@ -2896,11 +2912,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E86"/>
+  <dimension ref="A1:E87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A75" sqref="A75:XFD75"/>
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2954,7 +2970,7 @@
         <v>82734800</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="3" customFormat="1" ht="28">
@@ -2971,7 +2987,7 @@
         <v>42304</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="3" customFormat="1" ht="28">
@@ -2988,7 +3004,7 @@
         <v>105</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="3" customFormat="1" ht="28">
@@ -3005,7 +3021,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="3" customFormat="1" ht="28">
@@ -3022,7 +3038,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -3045,7 +3061,7 @@
         <v>158</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -3068,7 +3084,7 @@
         <v>201</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -3094,7 +3110,7 @@
         <v>122</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="42">
@@ -3111,7 +3127,7 @@
         <v>123</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="42">
@@ -3128,7 +3144,7 @@
         <v>124</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="70">
@@ -3145,7 +3161,7 @@
         <v>125</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="56">
@@ -3162,7 +3178,7 @@
         <v>126</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="70">
@@ -3179,7 +3195,7 @@
         <v>120</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="3" customFormat="1" ht="56">
@@ -3196,7 +3212,7 @@
         <v>127</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="56">
@@ -3213,7 +3229,7 @@
         <v>41444812</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="56">
@@ -3230,7 +3246,7 @@
         <v>120</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="56">
@@ -3247,7 +3263,7 @@
         <v>12345678</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="3" customFormat="1" ht="98">
@@ -3264,7 +3280,7 @@
         <v>8023631111</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="3" customFormat="1" ht="98">
@@ -3281,7 +3297,7 @@
         <v>8023631112</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="3" customFormat="1" ht="42">
@@ -3298,7 +3314,7 @@
         <v>24014</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="3" customFormat="1" ht="42">
@@ -3315,7 +3331,7 @@
         <v>128</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="3" customFormat="1" ht="56">
@@ -3332,7 +3348,7 @@
         <v>129</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="3" customFormat="1" ht="42">
@@ -3349,7 +3365,7 @@
         <v>130</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="3" customFormat="1" ht="42">
@@ -3360,7 +3376,7 @@
         <v>165</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="3" customFormat="1" ht="42">
@@ -3377,7 +3393,7 @@
         <v>135</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="3" customFormat="1" ht="42">
@@ -3388,7 +3404,7 @@
         <v>166</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="3" customFormat="1" ht="42">
@@ -3405,7 +3421,7 @@
         <v>131</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="3" customFormat="1" ht="42">
@@ -3422,7 +3438,7 @@
         <v>131</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -3448,7 +3464,7 @@
         <v>162</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="3" customFormat="1" ht="56">
@@ -3462,7 +3478,7 @@
         <v>132</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="3" customFormat="1" ht="56">
@@ -3479,7 +3495,7 @@
         <v>120</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="3" customFormat="1" ht="42">
@@ -3496,7 +3512,7 @@
         <v>2015</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="3" customFormat="1" ht="42">
@@ -3513,7 +3529,7 @@
         <v>134</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="3" customFormat="1" ht="42">
@@ -3530,7 +3546,7 @@
         <v>135</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="3" customFormat="1" ht="42">
@@ -3547,7 +3563,7 @@
         <v>136</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="3" customFormat="1" ht="42">
@@ -3564,7 +3580,7 @@
         <v>0</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
     </row>
     <row r="43" spans="1:5" s="3" customFormat="1" ht="56">
@@ -3581,7 +3597,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -3607,7 +3623,7 @@
         <v>121</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
     </row>
     <row r="46" spans="1:5" s="3" customFormat="1" ht="42">
@@ -3624,7 +3640,7 @@
         <v>137</v>
       </c>
       <c r="E46" s="15" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
     </row>
     <row r="47" spans="1:5" s="3" customFormat="1" ht="56">
@@ -3638,7 +3654,7 @@
         <v>28</v>
       </c>
       <c r="E47" s="15" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
     </row>
     <row r="48" spans="1:5" s="3" customFormat="1" ht="56">
@@ -3655,7 +3671,7 @@
         <v>139</v>
       </c>
       <c r="E48" s="15" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
     </row>
     <row r="49" spans="1:5" s="3" customFormat="1" ht="56">
@@ -3672,7 +3688,7 @@
         <v>140</v>
       </c>
       <c r="E49" s="15" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
     </row>
     <row r="50" spans="1:5" s="3" customFormat="1" ht="42">
@@ -3689,7 +3705,7 @@
         <v>141</v>
       </c>
       <c r="E50" s="15" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
     </row>
     <row r="51" spans="1:5" s="3" customFormat="1" ht="28">
@@ -3706,7 +3722,7 @@
         <v>0.2</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
     </row>
     <row r="52" spans="1:5" s="3" customFormat="1" ht="56">
@@ -3723,7 +3739,7 @@
         <v>30</v>
       </c>
       <c r="E52" s="15" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
     </row>
     <row r="53" spans="1:5" s="3" customFormat="1" ht="56">
@@ -3737,7 +3753,7 @@
         <v>164</v>
       </c>
       <c r="E53" s="15" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
     </row>
     <row r="54" spans="1:5" s="3" customFormat="1" ht="42">
@@ -3754,7 +3770,7 @@
         <v>40</v>
       </c>
       <c r="E54" s="15" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
     </row>
     <row r="55" spans="1:5" s="3" customFormat="1" ht="56">
@@ -3768,7 +3784,7 @@
         <v>164</v>
       </c>
       <c r="E55" s="15" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
     </row>
     <row r="56" spans="1:5" s="3" customFormat="1" ht="56">
@@ -3785,7 +3801,7 @@
         <v>0</v>
       </c>
       <c r="E56" s="15" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
     </row>
     <row r="57" spans="1:5" s="3" customFormat="1" ht="56">
@@ -3802,7 +3818,7 @@
         <v>0</v>
       </c>
       <c r="E57" s="15" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="58" spans="1:5" s="3" customFormat="1" ht="56">
@@ -3819,12 +3835,12 @@
         <v>0</v>
       </c>
       <c r="E58" s="15" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="56">
       <c r="A59" s="12" t="s">
-        <v>276</v>
+        <v>206</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>91</v>
@@ -3836,12 +3852,12 @@
         <v>1</v>
       </c>
       <c r="E59" s="15" t="s">
-        <v>280</v>
+        <v>264</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="56">
       <c r="A60" s="12" t="s">
-        <v>277</v>
+        <v>207</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>92</v>
@@ -3853,12 +3869,12 @@
         <v>1</v>
       </c>
       <c r="E60" s="15" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="56">
       <c r="A61" s="12" t="s">
-        <v>278</v>
+        <v>208</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>93</v>
@@ -3870,12 +3886,12 @@
         <v>1</v>
       </c>
       <c r="E61" s="15" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="56">
       <c r="A62" s="12" t="s">
-        <v>279</v>
+        <v>209</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>184</v>
@@ -3884,7 +3900,7 @@
         <v>87</v>
       </c>
       <c r="E62" s="15" t="s">
-        <v>283</v>
+        <v>267</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -3910,7 +3926,7 @@
         <v>143</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>257</v>
+        <v>268</v>
       </c>
     </row>
     <row r="65" spans="1:5" s="3" customFormat="1" ht="28">
@@ -3927,7 +3943,7 @@
         <v>142</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>258</v>
+        <v>269</v>
       </c>
     </row>
     <row r="66" spans="1:5" s="3" customFormat="1" ht="28">
@@ -3944,7 +3960,7 @@
         <v>144</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>259</v>
+        <v>270</v>
       </c>
     </row>
     <row r="67" spans="1:5" s="3" customFormat="1" ht="28">
@@ -3961,7 +3977,7 @@
         <v>145</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>260</v>
+        <v>271</v>
       </c>
     </row>
     <row r="68" spans="1:5" s="3" customFormat="1" ht="28">
@@ -3978,7 +3994,7 @@
         <v>0</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>261</v>
+        <v>272</v>
       </c>
     </row>
     <row r="69" spans="1:5" s="3" customFormat="1" ht="28">
@@ -3995,7 +4011,7 @@
         <v>2</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>262</v>
+        <v>273</v>
       </c>
     </row>
     <row r="70" spans="1:5" s="3" customFormat="1" ht="28">
@@ -4012,7 +4028,7 @@
         <v>47</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>263</v>
+        <v>274</v>
       </c>
     </row>
     <row r="71" spans="1:5" s="3" customFormat="1" ht="28">
@@ -4029,7 +4045,7 @@
         <v>1197</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>264</v>
+        <v>275</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -4055,208 +4071,225 @@
         <v>146</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>265</v>
+        <v>285</v>
       </c>
     </row>
     <row r="74" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A74" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" s="3" customFormat="1" ht="28">
+      <c r="A75" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B75" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C74" s="3" t="s">
+      <c r="C75" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D74" s="3">
+      <c r="D75" s="3">
         <v>12345</v>
       </c>
-      <c r="E74" s="3" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" s="3" customFormat="1" ht="42">
-      <c r="A75" s="3" t="s">
+      <c r="E75" s="3" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" s="3" customFormat="1" ht="42">
+      <c r="A76" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B76" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C75" s="3" t="s">
+      <c r="C76" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D75" s="3" t="s">
+      <c r="D76" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="E75" s="3" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" s="3" customFormat="1" ht="28">
-      <c r="A76" s="3" t="s">
+      <c r="E76" s="3" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" s="3" customFormat="1" ht="28">
+      <c r="A77" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B77" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C76" s="3" t="s">
+      <c r="C77" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D76" s="3" t="s">
+      <c r="D77" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="E76" s="3" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5">
-      <c r="A77" s="10" t="s">
+      <c r="E77" s="3" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="B77" s="5"/>
-      <c r="C77" s="5"/>
-      <c r="D77" s="5"/>
-      <c r="E77" s="5"/>
-    </row>
-    <row r="78" spans="1:5" ht="42">
-      <c r="A78" s="3" t="s">
+      <c r="B78" s="5"/>
+      <c r="C78" s="5"/>
+      <c r="D78" s="5"/>
+      <c r="E78" s="5"/>
+    </row>
+    <row r="79" spans="1:5" ht="42">
+      <c r="A79" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="B79" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C78" s="3" t="s">
+      <c r="C79" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D78" s="3" t="s">
+      <c r="D79" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="E78" s="3" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="42">
-      <c r="A79" s="14" t="s">
+      <c r="E79" s="3" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="42">
+      <c r="A80" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B80" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="C80" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D79" s="2" t="s">
+      <c r="D80" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="E79" s="3" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="56">
-      <c r="A80" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>150</v>
-      </c>
       <c r="E80" s="3" t="s">
-        <v>271</v>
+        <v>279</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="56">
       <c r="A81" s="3" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="56">
       <c r="A82" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>120</v>
+        <v>151</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="56">
       <c r="A83" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="56">
+      <c r="A84" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B83" s="3" t="s">
+      <c r="B84" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C83" s="3" t="s">
+      <c r="C84" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D83" s="3" t="s">
+      <c r="D84" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E83" s="3" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5">
-      <c r="A84" s="10" t="s">
+      <c r="E84" s="3" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="B84" s="5"/>
-      <c r="C84" s="5"/>
-      <c r="D84" s="5"/>
-      <c r="E84" s="5"/>
-    </row>
-    <row r="85" spans="1:5" ht="56">
-      <c r="A85" s="12" t="s">
+      <c r="B85" s="5"/>
+      <c r="C85" s="5"/>
+      <c r="D85" s="5"/>
+      <c r="E85" s="5"/>
+    </row>
+    <row r="86" spans="1:5" ht="56">
+      <c r="A86" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="B86" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="C85" s="2" t="s">
+      <c r="C86" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D85" s="2" t="b">
+      <c r="D86" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="E85" s="15" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="119" customHeight="1">
-      <c r="A86" s="17" t="s">
+      <c r="E86" s="15" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="119" customHeight="1">
+      <c r="A87" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="B86" s="18"/>
-      <c r="C86" s="18"/>
-      <c r="D86" s="18"/>
+      <c r="B87" s="18"/>
+      <c r="C87" s="18"/>
+      <c r="D87" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A86:D86"/>
+    <mergeCell ref="A87:D87"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Changed Officer Agency "ORI" to "Identification ID" in schema and mappings for the Incident Report and Court Filing IEPDs.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/service-specifications/Court_Case_Filing_Service/artifacts/service_model/information_model/Court_Case_Filing-IEPD/documentation/impl-artifacts/vermont/Citation_Case_Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/service-specifications/Court_Case_Filing_Service/artifacts/service_model/information_model/Court_Case_Filing-IEPD/documentation/impl-artifacts/vermont/Citation_Case_Mapping.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-28460" yWindow="5920" windowWidth="30440" windowHeight="15880"/>
+    <workbookView xWindow="-28455" yWindow="5925" windowWidth="29040" windowHeight="15885"/>
   </bookViews>
   <sheets>
     <sheet name="eCitation" sheetId="1" r:id="rId1"/>
@@ -435,9 +435,6 @@
     <t>1/1/2016:01:22</t>
   </si>
   <si>
-    <t>Officer Agency ORI</t>
-  </si>
-  <si>
     <t>Rt. 89</t>
   </si>
   <si>
@@ -851,9 +848,6 @@
     <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Offense/ojb-cit-ext:OffenseFineAmountMaximum</t>
   </si>
   <si>
-    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/j:CitationAgency/nc:OrganizationPrimaryContactInformation/nc:ContactEntity/ecf:EntityOrganization/j:OrganizationAugmentation/j:OrganizationORIIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
     <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/j:CitationAgency/nc:OrganizationName</t>
   </si>
   <si>
@@ -885,6 +879,12 @@
   </si>
   <si>
     <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/ojb-cit-ext:CitationIssuingOfficial/j:EnforcementOfficialBadgeIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>Officer Agency</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/j:CitationAgency/nc:OrganizationPrimaryContactInformation/nc:ContactEntity/ecf:EntityOrganization/nc:OrganizationIdentification/nc:IdentificationID</t>
   </si>
 </sst>
 </file>
@@ -892,7 +892,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -1849,7 +1849,7 @@
     <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2916,38 +2916,38 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C73" sqref="C73"/>
+      <selection pane="bottomLeft" activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.1640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="39.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="39.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="100.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="48.1640625" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="2"/>
+    <col min="4" max="4" width="21.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="100.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="48.140625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="9" customFormat="1" ht="28">
+    <row r="1" spans="1:5" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>119</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="19" customHeight="1">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>81</v>
       </c>
@@ -2956,29 +2956,29 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5" ht="28">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D3" s="2">
         <v>82734800</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="3" customFormat="1" ht="28">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>48</v>
@@ -2987,15 +2987,15 @@
         <v>42304</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="3" customFormat="1" ht="28">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>47</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>47</v>
@@ -3004,15 +3004,15 @@
         <v>105</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="3" customFormat="1" ht="28">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>49</v>
@@ -3021,15 +3021,15 @@
         <v>1</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="3" customFormat="1" ht="28">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>50</v>
@@ -3038,10 +3038,10 @@
         <v>0</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>62</v>
       </c>
@@ -3050,44 +3050,44 @@
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" ht="28">
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" ht="42">
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>63</v>
       </c>
@@ -3096,7 +3096,7 @@
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" ht="42">
+    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>64</v>
       </c>
@@ -3110,10 +3110,10 @@
         <v>122</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="42">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>2</v>
       </c>
@@ -3127,10 +3127,10 @@
         <v>123</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="42">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>94</v>
       </c>
@@ -3144,10 +3144,10 @@
         <v>124</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="70">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>57</v>
       </c>
@@ -3161,10 +3161,10 @@
         <v>125</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="56">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
@@ -3178,10 +3178,10 @@
         <v>126</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="70">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
@@ -3195,10 +3195,10 @@
         <v>120</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" s="3" customFormat="1" ht="56">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>6</v>
       </c>
@@ -3212,10 +3212,10 @@
         <v>127</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="56">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>1</v>
       </c>
@@ -3229,15 +3229,15 @@
         <v>41444812</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="56">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>90</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>8</v>
@@ -3246,10 +3246,10 @@
         <v>120</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="56">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>88</v>
       </c>
@@ -3263,15 +3263,15 @@
         <v>12345678</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" s="3" customFormat="1" ht="98">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>15</v>
@@ -3280,15 +3280,15 @@
         <v>8023631111</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" s="3" customFormat="1" ht="98">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>16</v>
@@ -3297,10 +3297,10 @@
         <v>8023631112</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" s="3" customFormat="1" ht="42">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>17</v>
       </c>
@@ -3314,10 +3314,10 @@
         <v>24014</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" s="3" customFormat="1" ht="42">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>65</v>
       </c>
@@ -3331,15 +3331,15 @@
         <v>128</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" s="3" customFormat="1" ht="56">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>18</v>
@@ -3348,10 +3348,10 @@
         <v>129</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" s="3" customFormat="1" ht="42">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>19</v>
       </c>
@@ -3365,21 +3365,21 @@
         <v>130</v>
       </c>
       <c r="E28" s="15" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E29" s="15" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="3" customFormat="1" ht="42">
-      <c r="A29" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="E29" s="15" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" s="3" customFormat="1" ht="42">
+    <row r="30" spans="1:5" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>20</v>
       </c>
@@ -3393,26 +3393,26 @@
         <v>135</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" s="3" customFormat="1" ht="42">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>116</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" s="3" customFormat="1" ht="42">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>21</v>
@@ -3421,15 +3421,15 @@
         <v>131</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" s="3" customFormat="1" ht="42">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>22</v>
@@ -3438,10 +3438,10 @@
         <v>131</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>84</v>
       </c>
@@ -3450,7 +3450,7 @@
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
     </row>
-    <row r="35" spans="1:5" s="3" customFormat="1" ht="42">
+    <row r="35" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>66</v>
       </c>
@@ -3461,13 +3461,13 @@
         <v>66</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" s="3" customFormat="1" ht="56">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>95</v>
       </c>
@@ -3478,15 +3478,15 @@
         <v>132</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" s="3" customFormat="1" ht="56">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>96</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>5</v>
@@ -3495,15 +3495,15 @@
         <v>120</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" s="3" customFormat="1" ht="42">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>97</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>23</v>
@@ -3512,15 +3512,15 @@
         <v>2015</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" s="3" customFormat="1" ht="42">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>98</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>24</v>
@@ -3529,15 +3529,15 @@
         <v>134</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" s="3" customFormat="1" ht="42">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>99</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>25</v>
@@ -3546,15 +3546,15 @@
         <v>135</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" s="3" customFormat="1" ht="42">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>100</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>26</v>
@@ -3563,15 +3563,15 @@
         <v>136</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" s="3" customFormat="1" ht="42">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>38</v>
@@ -3580,10 +3580,10 @@
         <v>0</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" s="3" customFormat="1" ht="56">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>101</v>
       </c>
@@ -3597,10 +3597,10 @@
         <v>0</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
         <v>82</v>
       </c>
@@ -3609,12 +3609,12 @@
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
     </row>
-    <row r="45" spans="1:5" s="3" customFormat="1" ht="68" customHeight="1">
+    <row r="45" spans="1:5" s="3" customFormat="1" ht="68.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
         <v>102</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>102</v>
@@ -3623,10 +3623,10 @@
         <v>121</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" s="3" customFormat="1" ht="42">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>103</v>
       </c>
@@ -3640,41 +3640,41 @@
         <v>137</v>
       </c>
       <c r="E46" s="15" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" s="3" customFormat="1" ht="56">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>104</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E47" s="15" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" s="3" customFormat="1" ht="56">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
         <v>105</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E48" s="15" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" s="3" customFormat="1" ht="56">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
         <v>106</v>
       </c>
@@ -3685,35 +3685,35 @@
         <v>30</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E49" s="15" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" s="3" customFormat="1" ht="42">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>107</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E50" s="15" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" s="3" customFormat="1" ht="28">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>108</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>32</v>
@@ -3722,10 +3722,10 @@
         <v>0.2</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" s="3" customFormat="1" ht="56">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>33</v>
       </c>
@@ -3739,24 +3739,24 @@
         <v>30</v>
       </c>
       <c r="E52" s="15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="E53" s="15" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="3" customFormat="1" ht="56">
-      <c r="A53" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="E53" s="15" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" s="3" customFormat="1" ht="42">
+    <row r="54" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>34</v>
       </c>
@@ -3770,24 +3770,24 @@
         <v>40</v>
       </c>
       <c r="E54" s="15" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="E55" s="15" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="55" spans="1:5" s="3" customFormat="1" ht="56">
-      <c r="A55" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="E55" s="15" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" s="3" customFormat="1" ht="56">
+    <row r="56" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>109</v>
       </c>
@@ -3801,10 +3801,10 @@
         <v>0</v>
       </c>
       <c r="E56" s="15" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" s="3" customFormat="1" ht="56">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>110</v>
       </c>
@@ -3818,10 +3818,10 @@
         <v>0</v>
       </c>
       <c r="E57" s="15" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" s="3" customFormat="1" ht="56">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>111</v>
       </c>
@@ -3835,12 +3835,12 @@
         <v>0</v>
       </c>
       <c r="E58" s="15" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="56">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>91</v>
@@ -3852,12 +3852,12 @@
         <v>1</v>
       </c>
       <c r="E59" s="15" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="56">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>92</v>
@@ -3869,12 +3869,12 @@
         <v>1</v>
       </c>
       <c r="E60" s="15" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="56">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>93</v>
@@ -3886,24 +3886,24 @@
         <v>1</v>
       </c>
       <c r="E61" s="15" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="56">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>87</v>
       </c>
       <c r="E62" s="15" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="s">
         <v>83</v>
       </c>
@@ -3912,24 +3912,24 @@
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
     </row>
-    <row r="64" spans="1:5" s="3" customFormat="1" ht="28">
+    <row r="64" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" s="3" customFormat="1" ht="28">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
         <v>112</v>
       </c>
@@ -3940,15 +3940,15 @@
         <v>40</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" s="3" customFormat="1" ht="28">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>76</v>
@@ -3957,13 +3957,13 @@
         <v>42</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" s="3" customFormat="1" ht="28">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>113</v>
       </c>
@@ -3974,18 +3974,18 @@
         <v>43</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" s="3" customFormat="1" ht="28">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>55</v>
@@ -3994,10 +3994,10 @@
         <v>0</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" s="3" customFormat="1" ht="28">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
         <v>114</v>
       </c>
@@ -4011,10 +4011,10 @@
         <v>2</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" s="3" customFormat="1" ht="28">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
         <v>117</v>
       </c>
@@ -4028,10 +4028,10 @@
         <v>47</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" s="3" customFormat="1" ht="28">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
         <v>118</v>
       </c>
@@ -4045,10 +4045,10 @@
         <v>1197</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
         <v>85</v>
       </c>
@@ -4057,7 +4057,7 @@
       <c r="D72" s="5"/>
       <c r="E72" s="5"/>
     </row>
-    <row r="73" spans="1:5" s="3" customFormat="1" ht="56">
+    <row r="73" spans="1:5" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>52</v>
       </c>
@@ -4068,30 +4068,30 @@
         <v>52</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" s="3" customFormat="1" ht="28">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B74" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="C74" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D74" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="C74" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>212</v>
-      </c>
       <c r="E74" s="3" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" s="3" customFormat="1" ht="28">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>115</v>
       </c>
@@ -4105,27 +4105,27 @@
         <v>12345</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" s="3" customFormat="1" ht="42">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>138</v>
+        <v>286</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>138</v>
+        <v>286</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" s="3" customFormat="1" ht="28">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>54</v>
       </c>
@@ -4136,13 +4136,13 @@
         <v>54</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="10" t="s">
         <v>86</v>
       </c>
@@ -4151,7 +4151,7 @@
       <c r="D78" s="5"/>
       <c r="E78" s="5"/>
     </row>
-    <row r="79" spans="1:5" ht="42">
+    <row r="79" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>2</v>
       </c>
@@ -4162,13 +4162,13 @@
         <v>2</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="42">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A80" s="14" t="s">
         <v>64</v>
       </c>
@@ -4182,10 +4182,10 @@
         <v>122</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" ht="56">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>57</v>
       </c>
@@ -4196,13 +4196,13 @@
         <v>57</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" ht="56">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>4</v>
       </c>
@@ -4213,13 +4213,13 @@
         <v>4</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" ht="56">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>5</v>
       </c>
@@ -4233,10 +4233,10 @@
         <v>120</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="56">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>6</v>
       </c>
@@ -4247,27 +4247,27 @@
         <v>6</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
       <c r="D85" s="5"/>
       <c r="E85" s="5"/>
     </row>
-    <row r="86" spans="1:5" ht="56">
+    <row r="86" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A86" s="12" t="s">
         <v>89</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>7</v>
@@ -4276,12 +4276,12 @@
         <v>0</v>
       </c>
       <c r="E86" s="15" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" ht="119" customHeight="1">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="119.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="17" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B87" s="18"/>
       <c r="C87" s="18"/>

</xml_diff>